<commit_message>
product backlog v5 e atualizacoes no planejamento matheus
</commit_message>
<xml_diff>
--- a/documentos/outros-documentos/Sprint-3/planejamento-sprint3.xlsx
+++ b/documentos/outros-documentos/Sprint-3/planejamento-sprint3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Id</t>
   </si>
@@ -63,22 +63,10 @@
     <t>Realizar testes</t>
   </si>
   <si>
-    <t>Estória de Usuário: CH:... ID:... – Mural de Serviços</t>
-  </si>
-  <si>
-    <t>Criar tela muralDeServicos</t>
-  </si>
-  <si>
-    <t>Com lista de serviços por categoria, botões Publicar no Mural e Minhas Publicações</t>
-  </si>
-  <si>
     <t>Criar controlador MuralDeServicosBean</t>
   </si>
   <si>
     <t>Criar classe de conexao com banco MuralDeServicosDAO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Com métodos listarServicosPorCategoria, publicarNoMural e listarPublicacoesUsuario </t>
   </si>
   <si>
     <t>De funcionalidade.</t>
@@ -91,9 +79,6 @@
   </si>
   <si>
     <t>Com atributos id, idUsuario, titulo, categoria, descricao. As anotaões servirão para criar as dependências entre objetos e a tabela no banco com os campos necessários.</t>
-  </si>
-  <si>
-    <t>Estória de Usuário: CH:... ID:... – Contato Usuário</t>
   </si>
   <si>
     <t>Refatorar parte Diagrama de classes Contato</t>
@@ -118,6 +103,24 @@
   </si>
   <si>
     <t>31/04/2016</t>
+  </si>
+  <si>
+    <t>Estória de Usuário: CH:2 ID:11 – Contatar Profissional</t>
+  </si>
+  <si>
+    <t>Estória de Usuário: CH:2 ID:11 – Publicar no Mural</t>
+  </si>
+  <si>
+    <t>Criar tela publicarNoMural</t>
+  </si>
+  <si>
+    <t>Com campos obrigatórios título, descricao e categoria que será uma lista das categoria do sistema. E o campo contato não obrigatório</t>
+  </si>
+  <si>
+    <t>Com método publicarNoMural passando por parametro o id da categoria selecionada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Com método publicarNoMural passando por parametro o id da categoria selecionada. </t>
   </si>
 </sst>
 </file>
@@ -842,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK905"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -862,7 +865,7 @@
   <sheetData>
     <row r="1" spans="1:1025" ht="15" thickBot="1">
       <c r="A1" s="29" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -974,12 +977,12 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:1025" s="3" customFormat="1" ht="39" thickBot="1">
+    <row r="4" spans="1:1025" s="3" customFormat="1" ht="77.25" thickBot="1">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>12</v>
@@ -994,7 +997,7 @@
         <v>42513</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="14"/>
@@ -1021,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
@@ -1036,7 +1039,7 @@
         <v>42514</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1063,13 +1066,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="11">
         <v>42515</v>
@@ -1078,7 +1081,7 @@
         <v>42515</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1105,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>12</v>
@@ -1120,7 +1123,7 @@
         <v>42515</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1162,7 +1165,7 @@
         <v>42516</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1254,7 +1257,7 @@
     </row>
     <row r="11" spans="1:1025" s="28" customFormat="1" ht="15" thickBot="1">
       <c r="A11" s="29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
@@ -3329,13 +3332,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E13" s="11">
         <v>42517</v>
@@ -4368,7 +4371,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>12</v>
@@ -4383,7 +4386,7 @@
         <v>42518</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="24"/>
@@ -5409,7 +5412,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>12</v>
@@ -5424,7 +5427,7 @@
         <v>42490</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="24"/>
@@ -6450,7 +6453,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>12</v>
@@ -6459,13 +6462,13 @@
         <v>7</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="24"/>
@@ -7506,7 +7509,7 @@
         <v>42491</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="24"/>

</xml_diff>